<commit_message>
As per the observations from ICON team post UAT, following changes have been made 1. Added city, state and country properties/fields to the SAM site 2. Additional sites web links were not appearing in the ICSF - Corrected 3. Country - India was missing in the Site Sources is Added 4. Add 'Additional Site' view is updated
</commit_message>
<xml_diff>
--- a/Documents/Technical/TestUpload/DDAS_Upload_CaseStudy_6.xlsx
+++ b/Documents/Technical/TestUpload/DDAS_Upload_CaseStudy_6.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="34">
   <si>
     <t>Project Number</t>
   </si>
@@ -70,9 +70,6 @@
     <t>Principal</t>
   </si>
   <si>
-    <t>0102/0304</t>
-  </si>
-  <si>
     <t>Apollo</t>
   </si>
   <si>
@@ -91,26 +88,41 @@
     <t>#6789</t>
   </si>
   <si>
-    <t>Bansal, Padam C. MD</t>
-  </si>
-  <si>
-    <t>Padam</t>
-  </si>
-  <si>
-    <t>Bansal</t>
-  </si>
-  <si>
     <t>0102</t>
   </si>
   <si>
-    <t>M#</t>
+    <t>PITISUTTIHUM Punnee</t>
+  </si>
+  <si>
+    <t>Punnee</t>
+  </si>
+  <si>
+    <t>PITISUTTIHUM</t>
+  </si>
+  <si>
+    <t>0000/0008</t>
+  </si>
+  <si>
+    <t>MACIAS-PARRA, MERCEDES</t>
+  </si>
+  <si>
+    <t>MERCEDES</t>
+  </si>
+  <si>
+    <t>MACIAS-PARRA</t>
+  </si>
+  <si>
+    <t>Punnee Pitisuttithum</t>
+  </si>
+  <si>
+    <t>Pitisuttithum</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -127,28 +139,18 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF333333"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF333333"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -186,7 +188,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -194,25 +196,31 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -515,10 +523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:Q7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -530,8 +538,8 @@
     <col min="5" max="5" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="24.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="22.140625" bestFit="1" customWidth="1"/>
@@ -613,52 +621,181 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="J2" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="K2" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" s="5"/>
+      <c r="M2" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="O2" s="6">
+        <v>889</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q2" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="C3" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="L3" s="5"/>
+      <c r="M3" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="N3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="O3" s="6">
+        <v>889</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q3" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="9"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="6"/>
+    </row>
+    <row r="5" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="9"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="6"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3" t="s">
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="I2" s="4" t="s">
+      <c r="H6" s="11"/>
+      <c r="I6" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J6" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="K6" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="L6" s="6"/>
+      <c r="M6" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="L2" s="4"/>
-      <c r="M2" s="6" t="s">
+      <c r="N6" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="O6" s="6">
+        <v>889</v>
+      </c>
+      <c r="P6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="O2" s="4">
-        <v>889</v>
-      </c>
-      <c r="P2" s="7" t="s">
+      <c r="Q6" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="Q2" s="4" t="s">
-        <v>24</v>
-      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D7" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
bug found. user name was not converted to lower case before validating.
</commit_message>
<xml_diff>
--- a/Documents/Technical/TestUpload/DDAS_Upload_CaseStudy_6.xlsx
+++ b/Documents/Technical/TestUpload/DDAS_Upload_CaseStudy_6.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Project Number</t>
   </si>
@@ -79,18 +79,6 @@
     <t>#6789</t>
   </si>
   <si>
-    <t>0102</t>
-  </si>
-  <si>
-    <t>PITISUTTIHUM Punnee</t>
-  </si>
-  <si>
-    <t>Punnee</t>
-  </si>
-  <si>
-    <t>PITISUTTIHUM</t>
-  </si>
-  <si>
     <t>0000/0008</t>
   </si>
   <si>
@@ -112,7 +100,10 @@
     <t>Role (PI/Sub I)</t>
   </si>
   <si>
-    <t>Sub I</t>
+    <t>Project Number 2</t>
+  </si>
+  <si>
+    <t>0000/8595</t>
   </si>
 </sst>
 </file>
@@ -185,7 +176,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -211,9 +202,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -520,191 +508,153 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q3"/>
+  <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="23" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="19.28515625" customWidth="1"/>
-    <col min="21" max="21" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="18.5703125" customWidth="1"/>
-    <col min="24" max="24" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="23" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.28515625" customWidth="1"/>
+    <col min="22" max="22" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="18.5703125" customWidth="1"/>
+    <col min="25" max="25" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="10">
+        <v>67873</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="L2" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="M2" s="5"/>
+      <c r="N2" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="P2" s="6">
+        <v>889</v>
+      </c>
+      <c r="Q2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="J2" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="K2" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="L2" s="5"/>
-      <c r="M2" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="O2" s="6">
-        <v>889</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q2" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="H3" s="11"/>
-      <c r="I3" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="J3" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="K3" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="L3" s="6"/>
-      <c r="M3" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="N3" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="O3" s="6">
-        <v>889</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q3" s="6" t="s">
+      <c r="R2" s="6" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>